<commit_message>
Finished p&l and CF quarters
</commit_message>
<xml_diff>
--- a/COIN.xlsx
+++ b/COIN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konst\valuations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3A9674-8413-47F5-BE07-68A237022429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9D1F72-989F-407D-96F5-901EC4E0E7F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="767" activeTab="5" xr2:uid="{A454576F-BA0E-4C95-85A1-1E0F525C6E61}"/>
   </bookViews>
@@ -228,9 +228,6 @@
     <t>Net income growth</t>
   </si>
   <si>
-    <t>Financing CF</t>
-  </si>
-  <si>
     <t>Currency</t>
   </si>
   <si>
@@ -445,6 +442,9 @@
   </si>
   <si>
     <t>calc.</t>
+  </si>
+  <si>
+    <t>FinCF</t>
   </si>
 </sst>
 </file>
@@ -1387,7 +1387,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1395,7 +1395,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1403,7 +1403,7 @@
         <v>21</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1411,7 +1411,7 @@
         <v>22</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1419,7 +1419,7 @@
         <v>18</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1432,23 +1432,23 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" s="43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F16">
         <v>2025</v>
@@ -1470,12 +1470,12 @@
         <v>2029</v>
       </c>
       <c r="K16" s="41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E18" s="39"/>
       <c r="F18" s="39"/>
@@ -1489,30 +1489,30 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E22" s="42"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E23" s="42"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" s="11"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E25" s="42"/>
     </row>
@@ -1545,8 +1545,8 @@
   </sheetPr>
   <dimension ref="A1:W762"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -1600,20 +1600,20 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
       <c r="R8" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S8" s="9"/>
       <c r="U8" s="34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="W8" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.2">
@@ -1622,52 +1622,52 @@
         <v>$m</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H9" s="32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I9" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K9" s="49" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L9" s="49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M9" s="49" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N9" s="49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O9" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="P9" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q9" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="P9" s="50" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q9" s="50" t="s">
-        <v>98</v>
-      </c>
       <c r="R9" s="50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S9" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U9" s="33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="2:23" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="2:23" x14ac:dyDescent="0.2">
       <c r="E11" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F11" s="17">
         <v>7839.4440000000004</v>
@@ -1717,7 +1717,7 @@
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.2">
       <c r="E12" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F12" s="16">
         <v>-1267.924</v>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.2">
       <c r="E13" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F13" s="16">
         <v>-1291.5609999999999</v>
@@ -1817,7 +1817,7 @@
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.2">
       <c r="E14" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F14" s="16">
         <v>-663.68899999999996</v>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.2">
       <c r="E15" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F15" s="16">
         <v>-909.39200000000005</v>
@@ -1917,7 +1917,7 @@
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.2">
       <c r="E16" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F16" s="16">
         <v>0</v>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="17" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E17" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F17" s="16">
         <v>-153.16</v>
@@ -2017,7 +2017,7 @@
     </row>
     <row r="18" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E18" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F18" s="16">
         <v>0</v>
@@ -2067,7 +2067,7 @@
     </row>
     <row r="19" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E19" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F19" s="18">
         <v>-477.14800000000002</v>
@@ -2117,7 +2117,7 @@
     </row>
     <row r="20" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E20" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F20" s="16">
         <f>SUM(F12:F19)</f>
@@ -2178,7 +2178,7 @@
     </row>
     <row r="21" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E21" s="44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F21" s="18">
         <v>-20.463000000000001</v>
@@ -2228,7 +2228,7 @@
     </row>
     <row r="22" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E22" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F22" s="17">
         <f>SUM(F11,F20:F21)</f>
@@ -2289,7 +2289,7 @@
     </row>
     <row r="23" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E23" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F23" s="16">
         <v>-29.16</v>
@@ -2339,7 +2339,7 @@
     </row>
     <row r="24" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E24" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F24" s="18">
         <v>0</v>
@@ -2675,7 +2675,7 @@
     </row>
     <row r="31" spans="5:21" x14ac:dyDescent="0.2">
       <c r="E31" s="37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F31" s="25">
         <f>-F26/F25</f>
@@ -2790,7 +2790,7 @@
     <row r="33" spans="3:21" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="3:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E34" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
@@ -2960,7 +2960,7 @@
       <c r="R39" s="9"/>
       <c r="S39" s="9"/>
       <c r="U39" s="34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="3:21" x14ac:dyDescent="0.2">
@@ -2969,52 +2969,52 @@
         <v>$m</v>
       </c>
       <c r="F40" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G40" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="G40" s="21" t="s">
+      <c r="H40" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="H40" s="21" t="s">
+      <c r="I40" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="I40" s="21" t="s">
-        <v>63</v>
-      </c>
       <c r="K40" s="49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L40" s="49" t="s">
         <v>28</v>
       </c>
       <c r="M40" s="49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N40" s="49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O40" s="50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P40" s="50" t="s">
         <v>29</v>
       </c>
       <c r="Q40" s="50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R40" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S40" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="U40" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="3:21" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E42" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F42" s="16">
         <v>988.19299999999998</v>
@@ -3052,7 +3052,7 @@
     </row>
     <row r="43" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E43" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F43" s="16">
         <f>625.758</f>
@@ -3094,7 +3094,7 @@
     </row>
     <row r="44" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E44" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F44" s="18">
         <f>98.385+59.23+952.307+176.689</f>
@@ -3137,7 +3137,7 @@
     </row>
     <row r="45" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E45" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F45" s="17">
         <f>SUM(F42:F44)</f>
@@ -3236,7 +3236,7 @@
     </row>
     <row r="47" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E47" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F47" s="16">
         <v>100.096</v>
@@ -3274,13 +3274,13 @@
     </row>
     <row r="48" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E48" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F48" s="47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G48" s="47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H48" s="16">
         <v>74.102999999999994</v>
@@ -3353,7 +3353,7 @@
     </row>
     <row r="50" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E50" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F50" s="18">
         <f>18373.863-SUM(F46:F49)</f>
@@ -3572,7 +3572,7 @@
     </row>
     <row r="55" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E55" s="45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F55" s="46">
         <v>3938</v>
@@ -3619,7 +3619,7 @@
     </row>
     <row r="56" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E56" s="45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F56" s="46">
         <f>SUM(F46:F47)</f>
@@ -3677,7 +3677,7 @@
     </row>
     <row r="57" spans="3:21" x14ac:dyDescent="0.2">
       <c r="E57" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F57" s="17">
         <f>+F55-F56</f>
@@ -3874,7 +3874,7 @@
       <c r="R62" s="9"/>
       <c r="S62" s="9"/>
       <c r="U62" s="34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="63" spans="3:21" x14ac:dyDescent="0.2">
@@ -3883,46 +3883,46 @@
         <v>$m</v>
       </c>
       <c r="F63" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G63" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="G63" s="21" t="s">
+      <c r="H63" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="H63" s="21" t="s">
+      <c r="I63" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="I63" s="21" t="s">
-        <v>63</v>
-      </c>
       <c r="K63" s="49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L63" s="49" t="s">
         <v>28</v>
       </c>
       <c r="M63" s="49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N63" s="49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O63" s="50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P63" s="50" t="s">
         <v>29</v>
       </c>
       <c r="Q63" s="50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R63" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S63" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="U63" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="64" spans="3:21" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3942,22 +3942,35 @@
       <c r="I65" s="16">
         <v>2556.8440000000001</v>
       </c>
-      <c r="K65" s="16"/>
-      <c r="L65" s="16"/>
+      <c r="K65" s="16">
+        <v>463.07799999999997</v>
+      </c>
+      <c r="L65" s="16">
+        <v>614.202</v>
+      </c>
       <c r="M65" s="16">
         <f>928.137-SUM(K65:L65)</f>
-        <v>928.13699999999994</v>
-      </c>
-      <c r="N65" s="16"/>
+        <v>-149.14300000000003</v>
+      </c>
+      <c r="N65" s="16">
+        <f>I65-SUM(K65:M65)</f>
+        <v>1628.7070000000001</v>
+      </c>
       <c r="O65" s="16">
         <v>411.48500000000001</v>
       </c>
-      <c r="P65" s="16"/>
+      <c r="P65" s="16">
+        <f>895.682-O65</f>
+        <v>484.197</v>
+      </c>
       <c r="Q65" s="16">
         <f>1592.226-SUM(O65:P65)</f>
-        <v>1180.741</v>
-      </c>
-      <c r="R65" s="16"/>
+        <v>696.5440000000001</v>
+      </c>
+      <c r="R65" s="16">
+        <f>I65-SUM(O65:Q65)</f>
+        <v>964.61799999999994</v>
+      </c>
       <c r="S65" s="16">
         <v>-182.727</v>
       </c>
@@ -3982,22 +3995,35 @@
       <c r="I66" s="18">
         <v>-282.38499999999999</v>
       </c>
-      <c r="K66" s="18"/>
-      <c r="L66" s="18"/>
+      <c r="K66" s="18">
+        <v>-26.08</v>
+      </c>
+      <c r="L66" s="18">
+        <v>-12.754</v>
+      </c>
       <c r="M66" s="18">
         <f>-85.117-SUM(K66:L66)</f>
-        <v>-85.117000000000004</v>
-      </c>
-      <c r="N66" s="18"/>
+        <v>-46.283000000000008</v>
+      </c>
+      <c r="N66" s="18">
+        <f>I66-SUM(K66:M66)</f>
+        <v>-197.26799999999997</v>
+      </c>
       <c r="O66" s="18">
         <v>-125.681</v>
       </c>
-      <c r="P66" s="18"/>
+      <c r="P66" s="18">
+        <f>-144.292-O66</f>
+        <v>-18.611000000000004</v>
+      </c>
       <c r="Q66" s="18">
         <f>-232.969-SUM(O66:P66)</f>
-        <v>-107.288</v>
-      </c>
-      <c r="R66" s="18"/>
+        <v>-88.676999999999992</v>
+      </c>
+      <c r="R66" s="18">
+        <f>I66-SUM(O66:Q66)</f>
+        <v>-49.415999999999997</v>
+      </c>
       <c r="S66" s="18">
         <v>-231.65299999999999</v>
       </c>
@@ -4028,19 +4054,19 @@
       </c>
       <c r="K67" s="17">
         <f t="shared" ref="K67:N67" si="67">+K65+K66</f>
-        <v>0</v>
+        <v>436.99799999999999</v>
       </c>
       <c r="L67" s="17">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>601.44799999999998</v>
       </c>
       <c r="M67" s="17">
         <f t="shared" si="67"/>
-        <v>843.02</v>
+        <v>-195.42600000000004</v>
       </c>
       <c r="N67" s="17">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>1431.4390000000001</v>
       </c>
       <c r="O67" s="17">
         <f>+O65+O66</f>
@@ -4048,15 +4074,15 @@
       </c>
       <c r="P67" s="17">
         <f>+P65+P66</f>
-        <v>0</v>
+        <v>465.58600000000001</v>
       </c>
       <c r="Q67" s="17">
         <f t="shared" ref="Q67:S67" si="68">+Q65+Q66</f>
-        <v>1073.453</v>
+        <v>607.86700000000008</v>
       </c>
       <c r="R67" s="17">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>915.202</v>
       </c>
       <c r="S67" s="17">
         <f t="shared" si="68"/>
@@ -4069,7 +4095,7 @@
     </row>
     <row r="68" spans="5:23" x14ac:dyDescent="0.2">
       <c r="E68" s="13" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="F68" s="16">
         <v>9976.0840000000007</v>
@@ -4083,22 +4109,35 @@
       <c r="I68" s="16">
         <v>2828.9209999999998</v>
       </c>
-      <c r="K68" s="16"/>
-      <c r="L68" s="16"/>
+      <c r="K68" s="16">
+        <v>460.12900000000002</v>
+      </c>
+      <c r="L68" s="16">
+        <v>-1142.2629999999999</v>
+      </c>
       <c r="M68" s="16">
         <f>-1734.128-SUM(K68:L68)</f>
-        <v>-1734.1279999999999</v>
-      </c>
-      <c r="N68" s="16"/>
+        <v>-1051.9940000000001</v>
+      </c>
+      <c r="N68" s="16">
+        <f>I68-SUM(K68:M68)</f>
+        <v>4563.049</v>
+      </c>
       <c r="O68" s="16">
         <v>1927.721</v>
       </c>
-      <c r="P68" s="16"/>
+      <c r="P68" s="16">
+        <f>993.988-O68</f>
+        <v>-933.73299999999995</v>
+      </c>
       <c r="Q68" s="16">
         <f>682.663-SUM(O68:P68)</f>
-        <v>-1245.058</v>
-      </c>
-      <c r="R68" s="16"/>
+        <v>-311.32500000000005</v>
+      </c>
+      <c r="R68" s="16">
+        <f>I68-SUM(O68:Q68)</f>
+        <v>2146.2579999999998</v>
+      </c>
       <c r="S68" s="16">
         <v>-893.80200000000002</v>
       </c>
@@ -4107,7 +4146,7 @@
         <v>-0.34301784391940782</v>
       </c>
       <c r="W68" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="71" spans="5:23" x14ac:dyDescent="0.2">
@@ -14509,9 +14548,9 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="F20:I20 K69:P209 S69:S209 K20:M68" formulaRange="1"/>
+    <ignoredError sqref="F20:I20 K69:P209 S69:S209 K20:M64 K67:M67 M65 M66 M68" formulaRange="1"/>
     <ignoredError sqref="Q210:R220" formula="1"/>
-    <ignoredError sqref="Q69:R209 S20:S68 N20:P68 Q20:R68" formula="1" formulaRange="1"/>
+    <ignoredError sqref="Q69:R209 S20:S68 N20:P64 Q20:R64 Q67:R67 Q65 Q66 Q68 N67:P67 O65 O66 O68" formula="1" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>